<commit_message>
Tue Mar 26 20:12:23 UTC 2024: update vbai-fhir
</commit_message>
<xml_diff>
--- a/vbai-fhir/StructureDefinition-vbai-body-height.xlsx
+++ b/vbai-fhir/StructureDefinition-vbai-body-height.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>2.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-26T03:52:16+00:00</t>
+    <t>2024-03-26T20:10:39+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Mon Apr 15 18:24:43 UTC 2024: update vbai-fhir
</commit_message>
<xml_diff>
--- a/vbai-fhir/StructureDefinition-vbai-body-height.xlsx
+++ b/vbai-fhir/StructureDefinition-vbai-body-height.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-26T20:10:39+00:00</t>
+    <t>2024-04-15T18:23:02+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,7 +72,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>KinD Lab (http://fhir.kindlab.sickkids.ca)</t>
   </si>
   <si>
     <t>Description</t>

</xml_diff>

<commit_message>
Tue Apr 16 16:31:58 UTC 2024: update vbai-fhir
</commit_message>
<xml_diff>
--- a/vbai-fhir/StructureDefinition-vbai-body-height.xlsx
+++ b/vbai-fhir/StructureDefinition-vbai-body-height.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.1</t>
+    <t>2.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-15T18:23:02+00:00</t>
+    <t>2024-04-16T16:30:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Mon May 13 19:45:11 UTC 2024: update vbai-fhir
</commit_message>
<xml_diff>
--- a/vbai-fhir/StructureDefinition-vbai-body-height.xlsx
+++ b/vbai-fhir/StructureDefinition-vbai-body-height.xlsx
@@ -27,13 +27,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://voicecollab.ai/fhir/StructureDefinition/vbai-body-height</t>
+    <t>https://kind-lab.github.io/vbai-fhir/StructureDefinition/vbai-body-height</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>2.1.0</t>
+    <t>2.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-16T16:30:12+00:00</t>
+    <t>2024-05-13T19:43:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -946,7 +946,7 @@
     <t>Observation.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://voicecollab.ai/fhir/StructureDefinition/vbai-patient)
+    <t xml:space="preserve">Reference(https://kind-lab.github.io/vbai-fhir/StructureDefinition/vbai-patient)
 </t>
   </si>
   <si>
@@ -1000,7 +1000,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://voicecollab.ai/fhir/StructureDefinition/vbai-encounter)
+    <t xml:space="preserve">Reference(https://kind-lab.github.io/vbai-fhir/StructureDefinition/vbai-encounter)
 </t>
   </si>
   <si>

</xml_diff>